<commit_message>
Merging Production Status to Github, Obtaining senior design files
</commit_message>
<xml_diff>
--- a/Airquality/Air_Quality_PnP.xlsx
+++ b/Airquality/Air_Quality_PnP.xlsx
@@ -456,11 +456,11 @@
   </sheetPr>
   <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F63" activeCellId="0" sqref="F63"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A66" activeCellId="0" sqref="A66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.98"/>
@@ -891,7 +891,7 @@
         <v>4</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>32.5</v>
+        <v>32.7</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>8</v>
@@ -911,10 +911,10 @@
         <v>29</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>1.95</v>
+        <v>1.5</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>29.55</v>
+        <v>29.8</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>8</v>
@@ -934,7 +934,7 @@
         <v>30</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>6.15</v>
+        <v>6.25</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>29.8</v>

</xml_diff>